<commit_message>
Added return to home page feature and improved design
</commit_message>
<xml_diff>
--- a/JNOrganizer.xlsx
+++ b/JNOrganizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoriav/Documents/JNOrganizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A6A368-D722-7646-92F1-E4414951FA14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF03A61-78C1-FF4E-AA2E-52DA1F3DD537}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="1160" windowWidth="22520" windowHeight="16320" xr2:uid="{7CA4D1F6-C442-8244-8318-9152705FDA58}"/>
+    <workbookView xWindow="5900" yWindow="1100" windowWidth="22520" windowHeight="16320" xr2:uid="{7CA4D1F6-C442-8244-8318-9152705FDA58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Creating JN Records app</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>terminate program - CTRL C</t>
+  </si>
+  <si>
+    <t>when wont let u use flask url</t>
+  </si>
+  <si>
+    <t>go to this link chrome://net-internals/#hsts</t>
+  </si>
+  <si>
+    <t>go to delete domain security policies</t>
+  </si>
+  <si>
+    <t>type in 127.0.0.1</t>
+  </si>
+  <si>
+    <t>delete and reload link</t>
   </si>
 </sst>
 </file>
@@ -469,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE61F11-F55B-574F-94BA-CCFE23698E4A}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,6 +621,29 @@
       <c r="B19" t="s">
         <v>25</v>
       </c>
+      <c r="L19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L23" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated dashboard design and fixed user home page
</commit_message>
<xml_diff>
--- a/JNOrganizer.xlsx
+++ b/JNOrganizer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoriav/Documents/JNOrganizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF03A61-78C1-FF4E-AA2E-52DA1F3DD537}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE398B6-316D-E448-9F13-B9B04222DA6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5900" yWindow="1100" windowWidth="22520" windowHeight="16320" xr2:uid="{7CA4D1F6-C442-8244-8318-9152705FDA58}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Creating JN Records app</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>delete and reload link</t>
+  </si>
+  <si>
+    <t>git status</t>
+  </si>
+  <si>
+    <t>git commit -m ""</t>
+  </si>
+  <si>
+    <t>git push origin main</t>
   </si>
 </sst>
 </file>
@@ -484,20 +493,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE61F11-F55B-574F-94BA-CCFE23698E4A}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -505,7 +514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45811</v>
       </c>
@@ -513,22 +522,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -536,54 +545,66 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="L10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="L11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="L12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>18</v>
       </c>
       <c r="L13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>20</v>
       </c>
@@ -591,7 +612,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Added feature to delete contracts from database
</commit_message>
<xml_diff>
--- a/JNOrganizer.xlsx
+++ b/JNOrganizer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoriav/Documents/JNOrganizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE398B6-316D-E448-9F13-B9B04222DA6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E94D90-E50E-5148-8F17-6BF7CED64139}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5900" yWindow="1100" windowWidth="22520" windowHeight="16320" xr2:uid="{7CA4D1F6-C442-8244-8318-9152705FDA58}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Creating JN Records app</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>git push origin main</t>
+  </si>
+  <si>
+    <t>chrome://settings/content/all</t>
+  </si>
+  <si>
+    <t>if site gets blocked</t>
   </si>
 </sst>
 </file>
@@ -496,7 +502,7 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,6 +617,9 @@
       <c r="L15" t="s">
         <v>27</v>
       </c>
+      <c r="P15" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
@@ -621,6 +630,9 @@
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
+      <c r="P16" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="3">

</xml_diff>